<commit_message>
added support for @CellFormat
This allows cells of type text or number, containing for example a
numeric identifier, to be bound to bean properties of String type.  The
cell format is used for the number values when converting to string.
</commit_message>
<xml_diff>
--- a/jawb-poi/src/test/resources/extractor-test.xlsx
+++ b/jawb-poi/src/test/resources/extractor-test.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="0" windowWidth="25600" windowHeight="16580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="25600" windowHeight="16580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" iterate="1" iterateCount="1" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -159,7 +159,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -214,7 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -234,13 +234,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -638,7 +639,7 @@
       </c>
       <c r="E2" s="2">
         <f ca="1">YEAR(TODAY()) - YEAR(F2)</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F2" s="1">
         <v>24910</v>
@@ -659,7 +660,7 @@
       </c>
       <c r="E3" s="2">
         <f ca="1">YEAR(TODAY()) - YEAR(F3)</f>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F3" s="1">
         <v>23202</v>
@@ -801,11 +802,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -814,6 +813,11 @@
     <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="6">
+        <v>905087030</v>
+      </c>
+    </row>
     <row r="2" spans="1:16">
       <c r="C2" t="s">
         <v>34</v>

</xml_diff>